<commit_message>
Funcs: add COUNTIFS and fix COUNTIF.
</commit_message>
<xml_diff>
--- a/samples/excel12/countif.xlsx
+++ b/samples/excel12/countif.xlsx
@@ -4,7 +4,7 @@
   <fileVersion lastEdited="4" lowestEdited="4" rupBuild="3820"/>
   <workbookPr date1904="0"/>
   <bookViews>
-    <workbookView activeTab="0" windowWidth="14400" windowHeight="5970"/>
+    <workbookView activeTab="0" windowWidth="14400" windowHeight="7790"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9" count="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11" count="11">
   <si>
     <t>Pass:</t>
   </si>
@@ -49,6 +49,12 @@
   </si>
   <si>
     <t>regexp</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
   <si>
     <t>String</t>
@@ -267,7 +273,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:IV18"/>
+  <dimension ref="A1:IV20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -289,7 +295,7 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <f t="array" ref="B1">SUM(0+B18:S18)</f>
+        <f t="array" ref="B1">SUM(0+B20:S20)</f>
         <v>18</v>
       </c>
     </row>
@@ -298,7 +304,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3">
-        <f>COLUMNS(B16:S18)-B1</f>
+        <f>COLUMNS(B18:S20)-B1</f>
         <v>0</v>
       </c>
     </row>
@@ -371,15 +377,11 @@
       <c r="C6" s="6">
         <v>1</v>
       </c>
-      <c r="D6" s="6" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E6" s="6" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="D6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="F6" s="6" t="b">
         <v>0</v>
@@ -408,7 +410,7 @@
         </is>
       </c>
       <c r="L6" s="6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="M6" s="6" t="s">
         <v>3</v>
@@ -933,7 +935,7 @@
       </c>
       <c r="B13">
         <f>COUNTIF($A13,B$6)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13">
         <f>COUNTIF($A13,C$6)</f>
@@ -941,7 +943,7 @@
       </c>
       <c r="D13">
         <f>COUNTIF($A13,D$6)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13">
         <f>COUNTIF($A13,E$6)</f>
@@ -973,11 +975,11 @@
       </c>
       <c r="L13">
         <f>COUNTIF($A13,L$6)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M13">
         <f>COUNTIF($A13,M$6)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N13">
         <f>COUNTIF($A13,N$6)</f>
@@ -989,7 +991,7 @@
       </c>
       <c r="P13">
         <f>COUNTIF($A13,P$6)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q13">
         <f>COUNTIF($A13,Q$6)</f>
@@ -997,224 +999,384 @@
       </c>
       <c r="R13">
         <f>COUNTIF($A13,R$6)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S13">
         <f>COUNTIF($A13,S$6)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U13">
         <f>2*U12</f>
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:256">
-      <c r="A16" t="s">
+    <row r="14" spans="1:256">
+      <c r="A14" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B16">
-        <f>SUMPRODUCT($U$7:$U$13,B7:B13)</f>
-        <v>1</v>
-      </c>
-      <c r="C16">
-        <f>SUMPRODUCT($U$7:$U$13,C7:C13)</f>
-        <v>2</v>
-      </c>
-      <c r="D16">
-        <f>SUMPRODUCT($U$7:$U$13,D7:D13)</f>
-        <v>1</v>
-      </c>
-      <c r="E16">
-        <f>SUMPRODUCT($U$7:$U$13,E7:E13)</f>
-        <v>2</v>
-      </c>
-      <c r="F16">
-        <f>SUMPRODUCT($U$7:$U$13,F7:F13)</f>
+      <c r="B14">
+        <f>COUNTIF($A14,B$6)</f>
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <f>COUNTIF($A14,C$6)</f>
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <f>COUNTIF($A14,D$6)</f>
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <f>COUNTIF($A14,E$6)</f>
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <f>COUNTIF($A14,F$6)</f>
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <f>COUNTIF($A14,G$6)</f>
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <f>COUNTIF($A14,H$6)</f>
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <f>COUNTIF($A14,I$6)</f>
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <f>COUNTIF($A14,J$6)</f>
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <f>COUNTIF($A14,K$6)</f>
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <f>COUNTIF($A14,L$6)</f>
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <f>COUNTIF($A14,M$6)</f>
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <f>COUNTIF($A14,N$6)</f>
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <f>COUNTIF($A14,O$6)</f>
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <f>COUNTIF($A14,P$6)</f>
+        <v>1</v>
+      </c>
+      <c r="Q14">
+        <f>COUNTIF($A14,Q$6)</f>
+        <v>1</v>
+      </c>
+      <c r="R14">
+        <f>COUNTIF($A14,R$6)</f>
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <f>COUNTIF($A14,S$6)</f>
+        <v>0</v>
+      </c>
+      <c r="U14">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="15" spans="1:256">
+      <c r="A15" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G16">
-        <f>SUMPRODUCT($U$7:$U$13,G7:G13)</f>
+      <c r="B15">
+        <f>COUNTIF($A15,B$6)</f>
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <f>COUNTIF($A15,C$6)</f>
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <f>COUNTIF($A15,D$6)</f>
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <f>COUNTIF($A15,E$6)</f>
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <f>COUNTIF($A15,F$6)</f>
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <f>COUNTIF($A15,G$6)</f>
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <f>COUNTIF($A15,H$6)</f>
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <f>COUNTIF($A15,I$6)</f>
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <f>COUNTIF($A15,J$6)</f>
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <f>COUNTIF($A15,K$6)</f>
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <f>COUNTIF($A15,L$6)</f>
+        <v>1</v>
+      </c>
+      <c r="M15">
+        <f>COUNTIF($A15,M$6)</f>
+        <v>1</v>
+      </c>
+      <c r="N15">
+        <f>COUNTIF($A15,N$6)</f>
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <f>COUNTIF($A15,O$6)</f>
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <f>COUNTIF($A15,P$6)</f>
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <f>COUNTIF($A15,Q$6)</f>
+        <v>1</v>
+      </c>
+      <c r="R15">
+        <f>COUNTIF($A15,R$6)</f>
+        <v>1</v>
+      </c>
+      <c r="S15">
+        <f>COUNTIF($A15,S$6)</f>
+        <v>0</v>
+      </c>
+      <c r="U15">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="18" spans="1:256">
+      <c r="A18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18">
+        <f>SUMPRODUCT($U$7:$U$15,B7:B15)</f>
+        <v>65</v>
+      </c>
+      <c r="C18">
+        <f>SUMPRODUCT($U$7:$U$15,C7:C15)</f>
+        <v>130</v>
+      </c>
+      <c r="D18">
+        <f>SUMPRODUCT($U$7:$U$15,D7:D15)</f>
+        <v>65</v>
+      </c>
+      <c r="E18">
+        <f>SUMPRODUCT($U$7:$U$15,E7:E15)</f>
+        <v>130</v>
+      </c>
+      <c r="F18">
+        <f>SUMPRODUCT($U$7:$U$15,F7:F15)</f>
+        <v>8</v>
+      </c>
+      <c r="G18">
+        <f>SUMPRODUCT($U$7:$U$15,G7:G15)</f>
         <v>16</v>
       </c>
-      <c r="H16">
-        <f>SUMPRODUCT($U$7:$U$13,H7:H13)</f>
+      <c r="H18">
+        <f>SUMPRODUCT($U$7:$U$15,H7:H15)</f>
         <v>8</v>
       </c>
-      <c r="I16">
-        <f>SUMPRODUCT($U$7:$U$13,I7:I13)</f>
+      <c r="I18">
+        <f>SUMPRODUCT($U$7:$U$15,I7:I15)</f>
         <v>16</v>
       </c>
-      <c r="J16">
-        <f>SUMPRODUCT($U$7:$U$13,J7:J13)</f>
-        <v>0</v>
-      </c>
-      <c r="K16">
-        <f>SUMPRODUCT($U$7:$U$13,K7:K13)</f>
-        <v>0</v>
-      </c>
-      <c r="L16">
-        <f>SUMPRODUCT($U$7:$U$13,L7:L13)</f>
+      <c r="J18">
+        <f>SUMPRODUCT($U$7:$U$15,J7:J15)</f>
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <f>SUMPRODUCT($U$7:$U$15,K7:K15)</f>
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <f>SUMPRODUCT($U$7:$U$15,L7:L15)</f>
+        <v>256</v>
+      </c>
+      <c r="M18">
+        <f>SUMPRODUCT($U$7:$U$15,M7:M15)</f>
+        <v>256</v>
+      </c>
+      <c r="N18">
+        <f>SUMPRODUCT($U$7:$U$15,N7:N15)</f>
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <f>SUMPRODUCT($U$7:$U$15,O7:O15)</f>
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <f>SUMPRODUCT($U$7:$U$15,P7:P15)</f>
+        <v>192</v>
+      </c>
+      <c r="Q18">
+        <f>SUMPRODUCT($U$7:$U$15,Q7:Q15)</f>
+        <v>448</v>
+      </c>
+      <c r="R18">
+        <f>SUMPRODUCT($U$7:$U$15,R7:R15)</f>
+        <v>256</v>
+      </c>
+      <c r="S18">
+        <f>SUMPRODUCT($U$7:$U$15,S7:S15)</f>
         <v>64</v>
       </c>
-      <c r="M16">
-        <f>SUMPRODUCT($U$7:$U$13,M7:M13)</f>
+    </row>
+    <row r="19" spans="1:256">
+      <c r="A19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19">
+        <v>65</v>
+      </c>
+      <c r="C19">
+        <v>130</v>
+      </c>
+      <c r="D19">
+        <v>65</v>
+      </c>
+      <c r="E19">
+        <v>130</v>
+      </c>
+      <c r="F19">
+        <v>8</v>
+      </c>
+      <c r="G19">
+        <v>16</v>
+      </c>
+      <c r="H19">
+        <v>8</v>
+      </c>
+      <c r="I19">
+        <v>16</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>256</v>
+      </c>
+      <c r="M19">
+        <v>256</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19">
+        <v>192</v>
+      </c>
+      <c r="Q19">
+        <v>448</v>
+      </c>
+      <c r="R19">
+        <v>256</v>
+      </c>
+      <c r="S19">
         <v>64</v>
       </c>
-      <c r="N16">
-        <f>SUMPRODUCT($U$7:$U$13,N7:N13)</f>
-        <v>0</v>
-      </c>
-      <c r="O16">
-        <f>SUMPRODUCT($U$7:$U$13,O7:O13)</f>
-        <v>0</v>
-      </c>
-      <c r="P16">
-        <f>SUMPRODUCT($U$7:$U$13,P7:P13)</f>
-        <v>0</v>
-      </c>
-      <c r="Q16">
-        <f>SUMPRODUCT($U$7:$U$13,Q7:Q13)</f>
-        <v>64</v>
-      </c>
-      <c r="R16">
-        <f>SUMPRODUCT($U$7:$U$13,R7:R13)</f>
-        <v>64</v>
-      </c>
-      <c r="S16">
-        <f>SUMPRODUCT($U$7:$U$13,S7:S13)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:256">
-      <c r="A17" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-      <c r="C17">
-        <v>2</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17">
-        <v>2</v>
-      </c>
-      <c r="F17">
-        <v>8</v>
-      </c>
-      <c r="G17">
-        <v>16</v>
-      </c>
-      <c r="H17">
-        <v>8</v>
-      </c>
-      <c r="I17">
-        <v>16</v>
-      </c>
-      <c r="J17">
-        <v>0</v>
-      </c>
-      <c r="K17">
-        <v>0</v>
-      </c>
-      <c r="L17">
-        <v>64</v>
-      </c>
-      <c r="M17">
-        <v>64</v>
-      </c>
-      <c r="N17">
-        <v>0</v>
-      </c>
-      <c r="O17">
-        <v>0</v>
-      </c>
-      <c r="P17">
-        <v>0</v>
-      </c>
-      <c r="Q17">
-        <v>64</v>
-      </c>
-      <c r="R17">
-        <v>64</v>
-      </c>
-      <c r="S17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:256">
-      <c r="B18" t="b">
-        <f>B16=B17</f>
-        <v>1</v>
-      </c>
-      <c r="C18" t="b">
-        <f>C16=C17</f>
-        <v>1</v>
-      </c>
-      <c r="D18" t="b">
-        <f>D16=D17</f>
-        <v>1</v>
-      </c>
-      <c r="E18" t="b">
-        <f>E16=E17</f>
-        <v>1</v>
-      </c>
-      <c r="F18" t="b">
-        <f>F16=F17</f>
-        <v>1</v>
-      </c>
-      <c r="G18" t="b">
-        <f>G16=G17</f>
-        <v>1</v>
-      </c>
-      <c r="H18" t="b">
-        <f>H16=H17</f>
-        <v>1</v>
-      </c>
-      <c r="I18" t="b">
-        <f>I16=I17</f>
-        <v>1</v>
-      </c>
-      <c r="J18" t="b">
-        <f>J16=J17</f>
-        <v>1</v>
-      </c>
-      <c r="K18" t="b">
-        <f>K16=K17</f>
-        <v>1</v>
-      </c>
-      <c r="L18" t="b">
-        <f>L16=L17</f>
-        <v>1</v>
-      </c>
-      <c r="M18" t="b">
-        <f>M16=M17</f>
-        <v>1</v>
-      </c>
-      <c r="N18" t="b">
-        <f>N16=N17</f>
-        <v>1</v>
-      </c>
-      <c r="O18" t="b">
-        <f>O16=O17</f>
-        <v>1</v>
-      </c>
-      <c r="P18" t="b">
-        <f>P16=P17</f>
-        <v>1</v>
-      </c>
-      <c r="Q18" t="b">
-        <f>Q16=Q17</f>
-        <v>1</v>
-      </c>
-      <c r="R18" t="b">
-        <f>R16=R17</f>
-        <v>1</v>
-      </c>
-      <c r="S18" t="b">
-        <f>S16=S17</f>
+    </row>
+    <row r="20" spans="1:256">
+      <c r="B20" t="b">
+        <f>B18=B19</f>
+        <v>1</v>
+      </c>
+      <c r="C20" t="b">
+        <f>C18=C19</f>
+        <v>1</v>
+      </c>
+      <c r="D20" t="b">
+        <f>D18=D19</f>
+        <v>1</v>
+      </c>
+      <c r="E20" t="b">
+        <f>E18=E19</f>
+        <v>1</v>
+      </c>
+      <c r="F20" t="b">
+        <f>F18=F19</f>
+        <v>1</v>
+      </c>
+      <c r="G20" t="b">
+        <f>G18=G19</f>
+        <v>1</v>
+      </c>
+      <c r="H20" t="b">
+        <f>H18=H19</f>
+        <v>1</v>
+      </c>
+      <c r="I20" t="b">
+        <f>I18=I19</f>
+        <v>1</v>
+      </c>
+      <c r="J20" t="b">
+        <f>J18=J19</f>
+        <v>1</v>
+      </c>
+      <c r="K20" t="b">
+        <f>K18=K19</f>
+        <v>1</v>
+      </c>
+      <c r="L20" t="b">
+        <f>L18=L19</f>
+        <v>1</v>
+      </c>
+      <c r="M20" t="b">
+        <f>M18=M19</f>
+        <v>1</v>
+      </c>
+      <c r="N20" t="b">
+        <f>N18=N19</f>
+        <v>1</v>
+      </c>
+      <c r="O20" t="b">
+        <f>O18=O19</f>
+        <v>1</v>
+      </c>
+      <c r="P20" t="b">
+        <f>P18=P19</f>
+        <v>1</v>
+      </c>
+      <c r="Q20" t="b">
+        <f>Q18=Q19</f>
+        <v>1</v>
+      </c>
+      <c r="R20" t="b">
+        <f>R18=R19</f>
+        <v>1</v>
+      </c>
+      <c r="S20" t="b">
+        <f>S18=S19</f>
         <v>1</v>
       </c>
     </row>
@@ -1235,7 +1397,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:IV18"/>
+  <dimension ref="A1:IV20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1253,7 +1415,7 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <f t="array" ref="B1">SUM(0+B18:G18)</f>
+        <f t="array" ref="B1">SUM(0+B20:G20)</f>
         <v>6</v>
       </c>
     </row>
@@ -1262,7 +1424,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3">
-        <f>COLUMNS(B16:G18)-B1</f>
+        <f>COLUMNS(B18:G20)-B1</f>
         <v>0</v>
       </c>
     </row>
@@ -1542,85 +1704,148 @@
         <v>0</v>
       </c>
       <c r="J13">
-        <f>2*J12</f>
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:256">
-      <c r="A16" t="s">
+    <row r="14" spans="1:256">
+      <c r="A14" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B16">
-        <f>SUMPRODUCT($J$7:$J$13,B7:B13)</f>
-        <v>2</v>
-      </c>
-      <c r="C16">
-        <f>SUMPRODUCT($J$7:$J$13,C7:C13)</f>
+      <c r="B14">
+        <f>COUNTIF($A14,B$6)</f>
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <f>COUNTIF($A14,C$6)</f>
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <f>COUNTIF($A14,D$6)</f>
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <f>COUNTIF($A14,E$6)</f>
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <f>COUNTIF($A14,F$6)</f>
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <f>COUNTIF($A14,G$6)</f>
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="15" spans="1:256">
+      <c r="A15" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15">
+        <f>COUNTIF($A15,B$6)</f>
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <f>COUNTIF($A15,C$6)</f>
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <f>COUNTIF($A15,D$6)</f>
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <f>COUNTIF($A15,E$6)</f>
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <f>COUNTIF($A15,F$6)</f>
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <f>COUNTIF($A15,G$6)</f>
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="18" spans="1:256">
+      <c r="A18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18">
+        <f>SUMPRODUCT($J$7:$J$15,B7:B15)</f>
+        <v>130</v>
+      </c>
+      <c r="C18">
+        <f>SUMPRODUCT($J$7:$J$15,C7:C15)</f>
         <v>4</v>
       </c>
-      <c r="D16">
-        <f>SUMPRODUCT($J$7:$J$13,D7:D13)</f>
+      <c r="D18">
+        <f>SUMPRODUCT($J$7:$J$15,D7:D15)</f>
         <v>6</v>
       </c>
-      <c r="E16">
-        <f>SUMPRODUCT($J$7:$J$13,E7:E13)</f>
-        <v>125</v>
-      </c>
-      <c r="F16">
-        <f>SUMPRODUCT($J$7:$J$13,F7:F13)</f>
+      <c r="E18">
+        <f>SUMPRODUCT($J$7:$J$15,E7:E15)</f>
+        <v>509</v>
+      </c>
+      <c r="F18">
+        <f>SUMPRODUCT($J$7:$J$15,F7:F15)</f>
         <v>3</v>
       </c>
-      <c r="G16">
-        <f>SUMPRODUCT($J$7:$J$13,G7:G13)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:256">
-      <c r="A17" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17">
-        <v>2</v>
-      </c>
-      <c r="C17">
+      <c r="G18">
+        <f>SUMPRODUCT($J$7:$J$15,G7:G15)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:256">
+      <c r="A19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19">
+        <v>130</v>
+      </c>
+      <c r="C19">
         <v>4</v>
       </c>
-      <c r="D17">
+      <c r="D19">
         <v>6</v>
       </c>
-      <c r="E17">
-        <v>125</v>
-      </c>
-      <c r="F17">
+      <c r="E19">
+        <v>509</v>
+      </c>
+      <c r="F19">
         <v>3</v>
       </c>
-      <c r="G17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:256">
-      <c r="B18" t="b">
-        <f>B16=B17</f>
-        <v>1</v>
-      </c>
-      <c r="C18" t="b">
-        <f>C16=C17</f>
-        <v>1</v>
-      </c>
-      <c r="D18" t="b">
-        <f>D16=D17</f>
-        <v>1</v>
-      </c>
-      <c r="E18" t="b">
-        <f>E16=E17</f>
-        <v>1</v>
-      </c>
-      <c r="F18" t="b">
-        <f>F16=F17</f>
-        <v>1</v>
-      </c>
-      <c r="G18" t="b">
-        <f>G16=G17</f>
+      <c r="G19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:256">
+      <c r="B20" t="b">
+        <f>B18=B19</f>
+        <v>1</v>
+      </c>
+      <c r="C20" t="b">
+        <f>C18=C19</f>
+        <v>1</v>
+      </c>
+      <c r="D20" t="b">
+        <f>D18=D19</f>
+        <v>1</v>
+      </c>
+      <c r="E20" t="b">
+        <f>E18=E19</f>
+        <v>1</v>
+      </c>
+      <c r="F20" t="b">
+        <f>F18=F19</f>
+        <v>1</v>
+      </c>
+      <c r="G20" t="b">
+        <f>G18=G19</f>
         <v>1</v>
       </c>
     </row>
@@ -1921,7 +2146,7 @@
     </row>
     <row r="13" spans="1:256">
       <c r="A13" s="6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B13">
         <f>COUNTIF($A13,B$6)</f>
@@ -1954,7 +2179,7 @@
     </row>
     <row r="16" spans="1:256">
       <c r="A16" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B16">
         <f>SUMPRODUCT($J$7:$J$13,B7:B13)</f>
@@ -1983,7 +2208,7 @@
     </row>
     <row r="17" spans="1:256">
       <c r="A17" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -2328,7 +2553,7 @@
     </row>
     <row r="13" spans="1:256">
       <c r="A13" s="6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B13">
         <f>COUNTIF($A13,B$6)</f>
@@ -2361,7 +2586,7 @@
     </row>
     <row r="16" spans="1:256">
       <c r="A16" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B16">
         <f>SUMPRODUCT($J$7:$J$13,B7:B13)</f>
@@ -2390,7 +2615,7 @@
     </row>
     <row r="17" spans="1:256">
       <c r="A17" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B17">
         <v>64</v>

</xml_diff>